<commit_message>
Add rest of outputs
</commit_message>
<xml_diff>
--- a/Outputs/1. Budget/Grid Search/Output Files/100000/Output_16_17.xlsx
+++ b/Outputs/1. Budget/Grid Search/Output Files/100000/Output_16_17.xlsx
@@ -480,8 +480,10 @@
           <t>Required Level of Met Demand</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -501,7 +503,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>62564.2577959615</v>
+        <v>76290.61593337962</v>
       </c>
     </row>
     <row r="7">
@@ -26317,7 +26319,7 @@
         <v>91381.29470172945</v>
       </c>
       <c r="D2" t="n">
-        <v>91381.29470172945</v>
+        <v>91381.29470172944</v>
       </c>
       <c r="E2" t="n">
         <v>97172.46592738405</v>
@@ -26372,7 +26374,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>133100</v>
+        <v>133100.0000000001</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -26415,49 +26417,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>86005.92442515714</v>
+        <v>86005.92442515712</v>
       </c>
       <c r="C4" t="n">
-        <v>86005.92442515714</v>
+        <v>86005.92442515712</v>
       </c>
       <c r="D4" t="n">
-        <v>86005.92442515714</v>
+        <v>86005.92442515712</v>
       </c>
       <c r="E4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="F4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="G4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="H4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="I4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="J4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="K4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="L4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="M4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="N4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="O4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
       <c r="P4" t="n">
-        <v>50967.55200287979</v>
+        <v>50967.5520028798</v>
       </c>
     </row>
     <row r="5">
@@ -26519,49 +26521,49 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-28252.22972342768</v>
+        <v>-28252.22972342767</v>
       </c>
       <c r="C6" t="n">
-        <v>-28252.22972342768</v>
+        <v>-28252.22972342767</v>
       </c>
       <c r="D6" t="n">
         <v>-28252.22972342768</v>
       </c>
       <c r="E6" t="n">
-        <v>-90506.69818050406</v>
+        <v>-90506.69818050413</v>
       </c>
       <c r="F6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="G6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="H6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="I6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="J6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="K6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="L6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="M6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="N6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="O6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
       <c r="P6" t="n">
-        <v>42593.30181949594</v>
+        <v>42593.30181949593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>